<commit_message>
Update Example benchmark.xlsx again
</commit_message>
<xml_diff>
--- a/Example benchmark.xlsx
+++ b/Example benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariusshekow/PycharmProjects/kubernetes-performance-benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4637E73C-3D19-494F-BB05-62870712F763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F90CC1-C3DB-1E47-AE88-FD943946AB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21640" activeTab="3" xr2:uid="{AFB2BC95-66F1-C647-8C60-6E45C53D1E86}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21640" xr2:uid="{AFB2BC95-66F1-C647-8C60-6E45C53D1E86}"/>
   </bookViews>
   <sheets>
     <sheet name="Results Disk (MBps)" sheetId="7" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="54">
   <si>
     <t>d4dsv5ephe</t>
   </si>
@@ -215,6 +215,15 @@
   </si>
   <si>
     <t>Price-Performance-Score</t>
+  </si>
+  <si>
+    <t>Standard_D4ds_v5 with Ephemeral OS disk</t>
+  </si>
+  <si>
+    <t>Standard_D3_v2 with managed disk</t>
+  </si>
+  <si>
+    <t>Other meta-data</t>
   </si>
 </sst>
 </file>
@@ -1769,14 +1778,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Meta-data'!$A$3:$A$4</c:f>
+              <c:f>'Meta-data'!$L$3:$L$4</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>d4dsv5ephe</c:v>
+                  <c:v>Standard_D4ds_v5 with Ephemeral OS disk</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>d3v2managed</c:v>
+                  <c:v>Standard_D3_v2 with managed disk</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4714,7 +4723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3695CD7A-EB44-C944-8B2F-E3DC64AF792A}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -6248,10 +6257,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32E1507-3665-9349-831E-2B51F08BBC5C}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6265,17 +6274,18 @@
     <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" customWidth="1"/>
-    <col min="13" max="13" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G1"/>
       <c r="H1"/>
       <c r="K1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -6312,8 +6322,12 @@
       <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M2" s="1"/>
+      <c r="N2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -6339,7 +6353,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="2">
-        <f>G3*$N$3+H3</f>
+        <f>G3*$O$3+H3</f>
         <v>198.56</v>
       </c>
       <c r="J3">
@@ -6350,14 +6364,17 @@
         <f>J3/I3</f>
         <v>4.9329741185994855E-2</v>
       </c>
-      <c r="M3" t="s">
+      <c r="L3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" t="s">
         <v>10</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>730</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -6383,7 +6400,7 @@
         <v>9.6</v>
       </c>
       <c r="I4" s="2">
-        <f>G4*$N$3+H4</f>
+        <f>G4*$O$3+H4</f>
         <v>208.16</v>
       </c>
       <c r="J4">
@@ -6394,11 +6411,14 @@
         <f>J4/I4</f>
         <v>9.6079938508839349E-3</v>
       </c>
-      <c r="M4" t="s">
+      <c r="L4" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" t="s">
         <v>15</v>
       </c>
-      <c r="N4">
-        <f>N3/24</f>
+      <c r="O4">
+        <f>O3/24</f>
         <v>30.416666666666668</v>
       </c>
     </row>

</xml_diff>